<commit_message>
added cursor size preview + steps to prefabricated parts
</commit_message>
<xml_diff>
--- a/imgs/zeitplan.xlsx
+++ b/imgs/zeitplan.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,127 +552,199 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_BA. 1_HFT_HFT setz.</t>
+          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_Beton_BET</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>HFT setz.</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>44952</v>
+        <v>44960</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44954</v>
+        <v>44961</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_Beton_BET</t>
+          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_Beton_BEW</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BET</t>
+          <t>BEW</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
+        <v>44958</v>
+      </c>
+      <c r="D8" s="2" t="n">
         <v>44960</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>44961</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_Beton_BEW</t>
+          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_Beton_Fertig</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BEW</t>
+          <t>Fertig</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>44958</v>
+        <v>44963</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>44960</v>
+        <v>44964</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_Beton_Fertig</t>
+          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_Beton_SCH</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fertig</t>
+          <t>SCH</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>44963</v>
+        <v>44957</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>44964</v>
+        <v>44959</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_Beton_SCH</t>
+          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_HFT_Fertig</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SCH</t>
+          <t>Fertig</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>44957</v>
+        <v>44963</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>44959</v>
+        <v>44964</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_HFT_Fertig</t>
+          <t>3_5_T1_SP_GRU_OG1_4101_03_F-P-001 - Decke_Kein BA_Beton_BET</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fertig</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>44963</v>
+        <v>44950</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>44964</v>
+        <v>44951</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Decke_BA. 1_HFT_HFT setz.</t>
+          <t>3_5_T1_SP_GRU_OG1_4101_03_F-P-001 - Decke_Kein BA_Beton_BEW</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>HFT setz.</t>
+          <t>BEW</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>44959</v>
+        <v>44949</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>44960</v>
+        <v>44950</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>3_5_T1_SP_GRU_OG1_4101_03_F-P-001 - Decke_Kein BA_Beton_SCH</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SCH</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>44946</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>44947</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>3_5_T1_SP_GRU_OG1_4101_03_F-P-001 - Decke_Kein BA_HFT_BET</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BET</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>44950</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>3_5_T1_SP_GRU_OG1_4101_03_F-P-001 - Decke_Kein BA_HFT_BEW</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BEW</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>44949</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>44950</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>3_5_T1_SP_GRU_OG1_4101_03_F-P-001 - Decke_Kein BA_HFT_HFT</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>HFT</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>44946</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>44947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed text-location, added floor planning, part complete stays for the whole time, new event only visible on one day
</commit_message>
<xml_diff>
--- a/imgs/zeitplan.xlsx
+++ b/imgs/zeitplan.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,19 +462,73 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_BA. 1_STB_SCH</t>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_STB_BET</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>BET</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45003</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_STB_BEW</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BEW</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>44999</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_STB_Fertig</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Fertig</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>44998</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45006</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_STB_SCH</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>SCH</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>44992</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>44993</v>
+      <c r="C5" s="2" t="n">
+        <v>44997</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>44998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 30 tacts+improved ui for legeng by printing
</commit_message>
<xml_diff>
--- a/imgs/zeitplan.xlsx
+++ b/imgs/zeitplan.xlsx
@@ -474,7 +474,7 @@
         <v>45009</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45010</v>
+        <v>45029</v>
       </c>
     </row>
     <row r="3">
@@ -492,7 +492,7 @@
         <v>45008</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45009</v>
+        <v>45028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
printing rows of rectangulars
</commit_message>
<xml_diff>
--- a/imgs/zeitplan.xlsx
+++ b/imgs/zeitplan.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,54 +462,90 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Erde</t>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Betonieren</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Beton@Erde</t>
+          <t>Beton@Betonieren</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45049</v>
+        <v>45051</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45050</v>
+        <v>45052</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Schalen</t>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Bewehren</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Beton@Schalen</t>
+          <t>Beton@Bewehren</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45050</v>
+        <v>45052</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45051</v>
+        <v>45053</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Erde</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Beton@Erde</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45049</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45050</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Schalen</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Beton@Schalen</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45050</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45051</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Vorbereitung</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Beton@Vorbereitung</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C6" s="2" t="n">
         <v>45048</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D6" s="2" t="n">
         <v>45049</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed tacts attributes bug+part complete after concrete
</commit_message>
<xml_diff>
--- a/imgs/zeitplan.xlsx
+++ b/imgs/zeitplan.xlsx
@@ -462,7 +462,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Erde</t>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_BA_1_Beton@Erde</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -480,7 +480,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Schalen</t>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_BA_1_Beton@Schalen</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -492,13 +492,13 @@
         <v>45050</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45051</v>
+        <v>45090</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_Kein BA_Beton@Vorbereitung</t>
+          <t>0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand_BA_1_Beton@Vorbereitung</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">

</xml_diff>